<commit_message>
add xlsx to json parsing
</commit_message>
<xml_diff>
--- a/jsonToXlsx/output.xlsx
+++ b/jsonToXlsx/output.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -387,6 +387,9 @@
       <c r="B1" t="str">
         <v>age</v>
       </c>
+      <c r="C1" t="str">
+        <v>nickname</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -395,6 +398,9 @@
       <c r="B2">
         <v>22</v>
       </c>
+      <c r="C2" t="str">
+        <v>aa's nickname</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -403,6 +409,9 @@
       <c r="B3">
         <v>33</v>
       </c>
+      <c r="C3" t="str">
+        <v>bb's nickname</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -411,6 +420,9 @@
       <c r="B4">
         <v>44</v>
       </c>
+      <c r="C4" t="str">
+        <v>cc's nickname</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -419,10 +431,13 @@
       <c r="B5">
         <v>55</v>
       </c>
+      <c r="C5" t="str">
+        <v>dd's nickname</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>